<commit_message>
progetto linguaggi parte B, completato lalr
</commit_message>
<xml_diff>
--- a/Bruniera/linguaggi e compilatori/progetto/parteB/lalr.xlsx
+++ b/Bruniera/linguaggi e compilatori/progetto/parteB/lalr.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>ACTION</t>
   </si>
@@ -66,118 +66,127 @@
     <t>I0</t>
   </si>
   <si>
+    <t>s3</t>
+  </si>
+  <si>
+    <t>s2</t>
+  </si>
+  <si>
+    <t>I1</t>
+  </si>
+  <si>
     <t>acc</t>
   </si>
   <si>
-    <t>e1</t>
-  </si>
-  <si>
-    <t>e2</t>
-  </si>
-  <si>
-    <t>e3</t>
-  </si>
-  <si>
-    <t>I1</t>
-  </si>
-  <si>
     <t>I2</t>
   </si>
   <si>
+    <t>r1</t>
+  </si>
+  <si>
     <t>I3</t>
   </si>
   <si>
+    <t>s6</t>
+  </si>
+  <si>
+    <t>s7</t>
+  </si>
+  <si>
     <t>I4</t>
   </si>
   <si>
+    <t>s9</t>
+  </si>
+  <si>
+    <t>s8</t>
+  </si>
+  <si>
     <t>I5</t>
   </si>
   <si>
+    <t>r6</t>
+  </si>
+  <si>
     <t>I6</t>
   </si>
   <si>
     <t>I7</t>
   </si>
   <si>
+    <t>r8</t>
+  </si>
+  <si>
     <t>I8</t>
   </si>
   <si>
+    <t>s13</t>
+  </si>
+  <si>
     <t>I9</t>
   </si>
   <si>
     <t>I10</t>
   </si>
   <si>
+    <t>s15</t>
+  </si>
+  <si>
     <t>I11</t>
   </si>
   <si>
+    <t>s16/r6</t>
+  </si>
+  <si>
+    <t>e6</t>
+  </si>
+  <si>
     <t>I12</t>
   </si>
   <si>
+    <t>s17</t>
+  </si>
+  <si>
     <t>I13</t>
   </si>
   <si>
     <t>I14</t>
   </si>
   <si>
+    <t>r5</t>
+  </si>
+  <si>
+    <t>s9/r5</t>
+  </si>
+  <si>
     <t>I15</t>
   </si>
   <si>
+    <t>r7</t>
+  </si>
+  <si>
     <t>I16</t>
   </si>
   <si>
+    <t>r9</t>
+  </si>
+  <si>
     <t>I17</t>
   </si>
   <si>
+    <t>r2</t>
+  </si>
+  <si>
     <t>I18</t>
   </si>
   <si>
+    <t>r3</t>
+  </si>
+  <si>
     <t>I19</t>
   </si>
   <si>
-    <t xml:space="preserve">print "internal error"; panic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">print "action outside of case"; drop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">print "expression outside of case"; drop</t>
-  </si>
-  <si>
-    <t>e4</t>
-  </si>
-  <si>
-    <t>e5</t>
-  </si>
-  <si>
-    <t>e6</t>
-  </si>
-  <si>
-    <t>e7</t>
-  </si>
-  <si>
-    <t>e8</t>
-  </si>
-  <si>
-    <t>e9</t>
-  </si>
-  <si>
-    <t>e10</t>
-  </si>
-  <si>
-    <t>e11</t>
-  </si>
-  <si>
-    <t>e12</t>
-  </si>
-  <si>
-    <t>e13</t>
-  </si>
-  <si>
-    <t>e14</t>
-  </si>
-  <si>
-    <t>e15</t>
+    <t>r4</t>
   </si>
 </sst>
 </file>
@@ -273,18 +282,17 @@
     <xf fontId="2" fillId="3" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="3" fillId="4" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="4" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf fontId="4" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf fontId="2" fillId="3" borderId="1" numFmtId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="1" fillId="2" borderId="1" numFmtId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="3" fillId="4" borderId="1" numFmtId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf fontId="2" fillId="3" borderId="1" numFmtId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -800,6 +808,12 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col customWidth="1" min="11" max="11" width="3.28125"/>
+    <col customWidth="1" min="12" max="12" width="3.140625"/>
+    <col customWidth="1" min="13" max="13" width="3.421875"/>
+    <col customWidth="1" min="14" max="15" width="3.28125"/>
+  </cols>
   <sheetData>
     <row r="2" ht="14.25">
       <c r="A2" s="1"/>
@@ -874,33 +888,26 @@
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="E4" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="G4" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L4" s="6">
+      <c r="K4" s="1"/>
+      <c r="L4" s="4">
         <v>1</v>
       </c>
-      <c r="M4" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="N4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>20</v>
-      </c>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
     </row>
     <row r="5" ht="14.25">
       <c r="A5" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -910,10 +917,10 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="J5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
@@ -921,20 +928,24 @@
     </row>
     <row r="6" ht="14.25">
       <c r="A6" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="F6" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="I6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
@@ -944,43 +955,46 @@
       <c r="A7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="B7" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="F7" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
-      <c r="K7" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
-      <c r="N7" s="6">
+      <c r="N7" s="4">
         <v>4</v>
       </c>
-      <c r="O7" s="6">
+      <c r="O7" s="4">
         <v>5</v>
       </c>
     </row>
     <row r="8" ht="14.25">
       <c r="A8" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="D8" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
+      <c r="H8" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
-      <c r="K8" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
@@ -988,20 +1002,23 @@
     </row>
     <row r="9" ht="14.25">
       <c r="A9" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
+      <c r="H9" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
-      <c r="K9" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
@@ -1009,45 +1026,51 @@
     </row>
     <row r="10" ht="14.25">
       <c r="A10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+      <c r="F10" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
-      <c r="K10" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
-      <c r="N10" s="6">
+      <c r="N10" s="4">
         <v>10</v>
       </c>
-      <c r="O10" s="6">
+      <c r="O10" s="4">
         <v>11</v>
       </c>
     </row>
     <row r="11" ht="14.25">
       <c r="A11" s="3" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="C11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
+      <c r="H11" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
-      <c r="K11" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
@@ -1055,22 +1078,22 @@
     </row>
     <row r="12" ht="14.25">
       <c r="A12" s="3" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="F12" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
-      <c r="K12" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="K12" s="1"/>
       <c r="L12" s="1"/>
-      <c r="M12" s="6">
+      <c r="M12" s="4">
         <v>12</v>
       </c>
       <c r="N12" s="1"/>
@@ -1078,45 +1101,49 @@
     </row>
     <row r="13" ht="14.25">
       <c r="A13" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="1"/>
+        <v>36</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="F13" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
-      <c r="K13" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
-      <c r="N13" s="6">
+      <c r="N13" s="4">
         <v>14</v>
       </c>
-      <c r="O13" s="6">
+      <c r="O13" s="4">
         <v>5</v>
       </c>
     </row>
     <row r="14" ht="14.25">
       <c r="A14" s="3" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
+      <c r="C14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
-      <c r="K14" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
@@ -1124,20 +1151,24 @@
     </row>
     <row r="15" ht="14.25">
       <c r="A15" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
+      <c r="C15" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
+      <c r="H15" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
-      <c r="K15" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
@@ -1145,20 +1176,19 @@
     </row>
     <row r="16" ht="14.25">
       <c r="A16" s="3" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
+      <c r="I16" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="J16" s="1"/>
-      <c r="K16" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
@@ -1166,21 +1196,23 @@
     </row>
     <row r="17" ht="14.25">
       <c r="A17" s="3" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="E17" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
+      <c r="G17" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
-      <c r="K17" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L17" s="6">
+      <c r="K17" s="1"/>
+      <c r="L17" s="4">
         <v>18</v>
       </c>
       <c r="M17" s="1"/>
@@ -1189,20 +1221,24 @@
     </row>
     <row r="18" ht="14.25">
       <c r="A18" s="3" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
+      <c r="C18" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
+      <c r="H18" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
-      <c r="K18" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
@@ -1210,20 +1246,24 @@
     </row>
     <row r="19" ht="14.25">
       <c r="A19" s="3" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
+      <c r="C19" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
+      <c r="H19" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
-      <c r="K19" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
@@ -1231,20 +1271,24 @@
     </row>
     <row r="20" ht="14.25">
       <c r="A20" s="3" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
+      <c r="C20" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
+      <c r="H20" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
-      <c r="K20" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
@@ -1252,20 +1296,24 @@
     </row>
     <row r="21" ht="14.25">
       <c r="A21" s="3" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
+      <c r="F21" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="I21" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
@@ -1273,22 +1321,24 @@
     </row>
     <row r="22" ht="14.25">
       <c r="A22" s="3" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
+      <c r="F22" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
+      <c r="I22" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="J22" s="1"/>
-      <c r="K22" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="K22" s="1"/>
       <c r="L22" s="1"/>
-      <c r="M22" s="6">
+      <c r="M22" s="4">
         <v>19</v>
       </c>
       <c r="N22" s="1"/>
@@ -1296,7 +1346,7 @@
     </row>
     <row r="23" ht="14.25">
       <c r="A23" s="3" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1305,11 +1355,11 @@
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
+      <c r="I23" s="4" t="s">
+        <v>57</v>
+      </c>
       <c r="J23" s="1"/>
-      <c r="K23" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
@@ -1322,100 +1372,64 @@
       <c r="A25" s="7"/>
     </row>
     <row r="26" ht="14.25">
-      <c r="A26" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>40</v>
-      </c>
+      <c r="A26"/>
+      <c r="B26"/>
     </row>
     <row r="27" ht="14.25">
-      <c r="A27" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>41</v>
-      </c>
+      <c r="A27"/>
+      <c r="B27"/>
     </row>
     <row r="28" ht="14.25">
-      <c r="A28" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>42</v>
-      </c>
+      <c r="A28"/>
+      <c r="B28"/>
     </row>
     <row r="29" ht="14.25">
-      <c r="A29" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B29" s="1"/>
+      <c r="A29"/>
+      <c r="B29"/>
     </row>
     <row r="30" ht="14.25">
-      <c r="A30" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B30" s="1"/>
+      <c r="A30"/>
+      <c r="B30"/>
     </row>
     <row r="31" ht="14.25">
-      <c r="A31" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B31" s="1"/>
+      <c r="A31"/>
+      <c r="B31"/>
     </row>
     <row r="32" ht="14.25">
-      <c r="A32" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B32" s="1"/>
+      <c r="A32"/>
+      <c r="B32"/>
     </row>
     <row r="33" ht="14.25">
-      <c r="A33" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B33" s="1"/>
+      <c r="A33"/>
+      <c r="B33"/>
     </row>
     <row r="34" ht="14.25">
-      <c r="A34" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B34" s="1"/>
+      <c r="A34"/>
+      <c r="B34"/>
     </row>
     <row r="35" ht="14.25">
-      <c r="A35" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B35" s="1"/>
+      <c r="A35"/>
+      <c r="B35"/>
     </row>
     <row r="36" ht="14.25">
-      <c r="A36" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B36" s="1"/>
+      <c r="A36"/>
+      <c r="B36"/>
     </row>
     <row r="37" ht="14.25">
-      <c r="A37" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B37" s="1"/>
+      <c r="A37"/>
+      <c r="B37"/>
     </row>
     <row r="38" ht="14.25">
-      <c r="A38" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B38" s="1"/>
+      <c r="A38"/>
+      <c r="B38"/>
     </row>
     <row r="39" ht="14.25">
-      <c r="A39" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B39" s="1"/>
+      <c r="A39"/>
+      <c r="B39"/>
     </row>
     <row r="40" ht="14.25">
-      <c r="A40" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B40" s="1"/>
+      <c r="A40"/>
+      <c r="B40"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>